<commit_message>
Enabling all testcase ECTEST KIT
</commit_message>
<xml_diff>
--- a/Input_files/Master_executors/ECTEST/KIT/MasterExecutor_Sanity.xlsx
+++ b/Input_files/Master_executors/ECTEST/KIT/MasterExecutor_Sanity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_Muitisite\Input_files\Master_executors\ECTEST\KIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633705D1-67F1-49F8-B221-7C1ACD409D7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D577070-E876-4DD4-847C-65CA15A87616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="66">
   <si>
     <t>Runmode</t>
   </si>
@@ -243,9 +243,6 @@
   </si>
   <si>
     <t>TC30_Verify_pagination_SortBy_filteronPLP</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
 </sst>
 </file>
@@ -775,7 +772,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E29"/>
+      <selection activeCell="E2" sqref="E2:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -841,7 +838,7 @@
         <v>17</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>10</v>
@@ -861,7 +858,7 @@
         <v>19</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>10</v>
@@ -881,7 +878,7 @@
         <v>13</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>10</v>
@@ -901,7 +898,7 @@
         <v>12</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>10</v>
@@ -921,7 +918,7 @@
         <v>11</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>10</v>
@@ -941,7 +938,7 @@
         <v>14</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>10</v>
@@ -961,7 +958,7 @@
         <v>23</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>10</v>
@@ -981,7 +978,7 @@
         <v>25</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>10</v>
@@ -1001,7 +998,7 @@
         <v>15</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>10</v>
@@ -1021,7 +1018,7 @@
         <v>28</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>10</v>
@@ -1041,7 +1038,7 @@
         <v>30</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>10</v>
@@ -1061,7 +1058,7 @@
         <v>32</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>10</v>
@@ -1081,7 +1078,7 @@
         <v>33</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>10</v>
@@ -1101,7 +1098,7 @@
         <v>35</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>10</v>
@@ -1121,7 +1118,7 @@
         <v>37</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>10</v>
@@ -1141,7 +1138,7 @@
         <v>39</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>10</v>
@@ -1161,7 +1158,7 @@
         <v>41</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>10</v>
@@ -1181,7 +1178,7 @@
         <v>43</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>10</v>
@@ -1201,7 +1198,7 @@
         <v>45</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>10</v>
@@ -1221,7 +1218,7 @@
         <v>47</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>10</v>
@@ -1241,7 +1238,7 @@
         <v>49</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>10</v>
@@ -1261,7 +1258,7 @@
         <v>51</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>10</v>
@@ -1281,7 +1278,7 @@
         <v>53</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>10</v>
@@ -1301,7 +1298,7 @@
         <v>55</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>10</v>
@@ -1321,7 +1318,7 @@
         <v>56</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>10</v>
@@ -1341,7 +1338,7 @@
         <v>58</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>10</v>
@@ -1361,7 +1358,7 @@
         <v>60</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Disabling TC26 & TC28 for KIT
</commit_message>
<xml_diff>
--- a/Input_files/Master_executors/ECTEST/KIT/MasterExecutor_Sanity.xlsx
+++ b/Input_files/Master_executors/ECTEST/KIT/MasterExecutor_Sanity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_Muitisite\Input_files\Master_executors\ECTEST\KIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93815853-4B3D-431F-AC17-75EED4245C64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B15E228-F186-4AE7-A9CA-CD91B13EC2A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="67">
   <si>
     <t>Runmode</t>
   </si>
@@ -243,6 +243,9 @@
   </si>
   <si>
     <t>TC30_Verify_pagination_SortBy_filteronPLP</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -771,8 +774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E29"/>
+    <sheetView tabSelected="1" topLeftCell="C19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1238,7 +1241,7 @@
         <v>49</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>10</v>
@@ -1278,7 +1281,7 @@
         <v>53</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>10</v>

</xml_diff>